<commit_message>
Add problem statement and solutions for filtering relevant dates based on day indicators
</commit_message>
<xml_diff>
--- a/Find_Relevant_Dates/Problem_Statement.xlsx
+++ b/Find_Relevant_Dates/Problem_Statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thoufiq/THOUFIQ/techTFQ/YouTube/VIDEOS/30 SQL Interview Queries/Video_Q7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\30DaySQLQueryChallenge - techTFQ\Find_Relevant_Dates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7242DB1E-9B31-F741-8CD8-C2A59502F976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF05DE9D-098F-4587-8FAC-0036C2756CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{0CBE3013-8546-5E45-9781-4A0E0588E0FC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{0CBE3013-8546-5E45-9781-4A0E0588E0FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -51,29 +49,6 @@
   </si>
   <si>
     <t>DATES</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Video #7 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Find Relevant dates</t>
-    </r>
   </si>
   <si>
     <r>
@@ -104,6 +79,29 @@
   </si>
   <si>
     <t>OUTPUT</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"># </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Find Relevant dates</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -430,23 +428,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -480,6 +463,21 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,87 +814,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FDD7B68-1CE0-4246-844B-4C52F096307A}">
   <dimension ref="B1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="4" width="15.83203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="1"/>
-    <col min="7" max="9" width="15.83203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.796875" style="1"/>
+    <col min="2" max="2" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.796875" style="1"/>
+    <col min="7" max="7" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="2:9" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="B1" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+    </row>
+    <row r="2" spans="2:9" s="4" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="2:9" s="5" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+    </row>
+    <row r="3" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+    </row>
+    <row r="4" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+    </row>
+    <row r="5" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+    </row>
+    <row r="6" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+    </row>
+    <row r="7" spans="2:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -906,252 +908,252 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+    <row r="8" spans="2:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
+      <c r="G8" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="G8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="H8" s="29"/>
+      <c r="I8" s="30"/>
+    </row>
+    <row r="9" spans="2:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="16" t="s">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="12">
         <v>1010101</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="13">
         <v>45355</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="12">
         <v>1010101</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="13">
         <v>45355</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="25" t="s">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="21">
         <v>1010101</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="22">
         <v>45356</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="H11" s="26">
+      <c r="H11" s="21">
         <v>1010101</v>
       </c>
-      <c r="I11" s="27">
+      <c r="I11" s="22">
         <v>45357</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="19" t="s">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="15">
         <v>1010101</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="16">
         <v>45357</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="15">
         <v>1010101</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="16">
         <v>45359</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="25" t="s">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="21">
         <v>1010101</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="22">
         <v>45358</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="H13" s="26">
+      <c r="H13" s="21">
         <v>1010101</v>
       </c>
-      <c r="I13" s="27">
+      <c r="I13" s="22">
         <v>45361</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="19" t="s">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="15">
         <v>1010101</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="16">
         <v>45359</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="15">
         <v>1000110</v>
       </c>
-      <c r="I14" s="21">
+      <c r="I14" s="16">
         <v>45355</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="25" t="s">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="21">
         <v>1010101</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="22">
         <v>45360</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="26">
+      <c r="H15" s="21">
         <v>1000110</v>
       </c>
-      <c r="I15" s="27">
+      <c r="I15" s="22">
         <v>45359</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="19" t="s">
+    <row r="16" spans="2:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="15">
         <v>1010101</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="16">
         <v>45361</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="18">
         <v>1000110</v>
       </c>
-      <c r="I16" s="24">
+      <c r="I16" s="19">
         <v>45360</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="25" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="21">
         <v>1000110</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="22">
         <v>45355</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="19" t="s">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="15">
         <v>1000110</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="16">
         <v>45356</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="25" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="21">
         <v>1000110</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="22">
         <v>45357</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="19" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="15">
         <v>1000110</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="16">
         <v>45358</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="25" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="21">
         <v>1000110</v>
       </c>
-      <c r="D21" s="27">
+      <c r="D21" s="22">
         <v>45359</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="19" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="15">
         <v>1000110</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="16">
         <v>45360</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="28" t="s">
+    <row r="23" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="29">
+      <c r="C23" s="24">
         <v>1000110</v>
       </c>
-      <c r="D23" s="30">
+      <c r="D23" s="25">
         <v>45361</v>
       </c>
     </row>
@@ -1163,5 +1165,6 @@
     <mergeCell ref="G8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>